<commit_message>
description to count working and loaded
</commit_message>
<xml_diff>
--- a/indeed_search_set.xlsx
+++ b/indeed_search_set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software\gnarfle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2924801D-96FA-4384-87BB-B705B383F054}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D292A4-AB89-45CF-A1E4-FA6375C17364}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4B06B630-D528-487E-B368-8826F295A53A}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4B06B630-D528-487E-B368-8826F295A53A}"/>
   </bookViews>
   <sheets>
     <sheet name="indeed_search_set" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>search_keyword_list</t>
   </si>
@@ -39,9 +39,6 @@
     <t>iss_pk</t>
   </si>
   <si>
-    <t>data analyst</t>
-  </si>
-  <si>
     <t>creation_date</t>
   </si>
   <si>
@@ -51,34 +48,46 @@
     <t>search_run_date</t>
   </si>
   <si>
-    <t>piano player</t>
-  </si>
-  <si>
-    <t>pizza delivery</t>
-  </si>
-  <si>
     <t>search_zip_code</t>
   </si>
   <si>
-    <t>python developer</t>
-  </si>
-  <si>
-    <t>19124</t>
-  </si>
-  <si>
-    <t>10018</t>
-  </si>
-  <si>
-    <t>90210</t>
-  </si>
-  <si>
-    <t>60606</t>
-  </si>
-  <si>
     <t>30303</t>
   </si>
   <si>
-    <t>75024</t>
+    <t>02109</t>
+  </si>
+  <si>
+    <t>10001</t>
+  </si>
+  <si>
+    <t>90021</t>
+  </si>
+  <si>
+    <t>60605</t>
+  </si>
+  <si>
+    <t>75202</t>
+  </si>
+  <si>
+    <t>77002</t>
+  </si>
+  <si>
+    <t>20004</t>
+  </si>
+  <si>
+    <t>19102</t>
+  </si>
+  <si>
+    <t>33131</t>
+  </si>
+  <si>
+    <t>85003</t>
+  </si>
+  <si>
+    <t>94111</t>
+  </si>
+  <si>
+    <t>python+tableau</t>
   </si>
 </sst>
 </file>
@@ -434,7 +443,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,16 +463,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -471,13 +480,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1">
-        <v>43715</v>
+        <v>43720</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -488,33 +497,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1">
-        <v>43715</v>
+        <v>43720</v>
       </c>
       <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>43715</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1">
-        <v>43715</v>
+        <v>43720</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -525,13 +532,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="1">
-        <v>43715</v>
+        <v>43720</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -542,13 +549,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="1">
-        <v>43715</v>
+        <v>43720</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -559,13 +566,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="1">
-        <v>43715</v>
+        <v>43720</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -576,13 +583,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="1">
-        <v>43715</v>
+        <v>43720</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -593,13 +600,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1">
-        <v>43715</v>
+        <v>43720</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -610,13 +617,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D10" s="1">
-        <v>43715</v>
+        <v>43720</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -627,13 +634,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1">
-        <v>43715</v>
+        <v>43720</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -644,13 +651,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1">
-        <v>43715</v>
+        <v>43720</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -661,34 +668,20 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1">
-        <v>43715</v>
+        <v>43720</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1">
-        <v>43715</v>
-      </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
+      <c r="D14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>